<commit_message>
Scheels label improvement and some chewy improvement
</commit_message>
<xml_diff>
--- a/assets/Scheels/Blank Scheels 856 ASN.xlsx
+++ b/assets/Scheels/Blank Scheels 856 ASN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cloudconvert\server\files\tasks\b8cb639b-550e-4a2f-a3c5-c8fdebe3a9fb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf-my.sharepoint.com/personal/gabbye_petreleaf_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4ECDC65-53BE-45E3-AB46-66DCE5E21C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{B4ECDC65-53BE-45E3-AB46-66DCE5E21C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C051FF-2DAA-4C24-9432-FEDA96F91B5C}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14400" windowHeight="8235"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Shipment #</t>
   </si>
@@ -44,15 +44,6 @@
     <t>Total Weight</t>
   </si>
   <si>
-    <t>12 Digit</t>
-  </si>
-  <si>
-    <t>UPC Number</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -65,9 +56,6 @@
     <t>Ship From Add1</t>
   </si>
   <si>
-    <t>Ship From Add2</t>
-  </si>
-  <si>
     <t>Ship From City</t>
   </si>
   <si>
@@ -98,9 +86,6 @@
     <t>Ship To Add1</t>
   </si>
   <si>
-    <t>Ship To Add2</t>
-  </si>
-  <si>
     <t>Ship To City</t>
   </si>
   <si>
@@ -125,9 +110,6 @@
     <t>Shipment Type</t>
   </si>
   <si>
-    <t>C - Cartons or P -Pallets</t>
-  </si>
-  <si>
     <t>Vendor #</t>
   </si>
   <si>
@@ -137,9 +119,6 @@
     <t>FOB</t>
   </si>
   <si>
-    <t>CC - Collect or PP - Prepaid</t>
-  </si>
-  <si>
     <t>Total Cartons / Pallets</t>
   </si>
   <si>
@@ -164,12 +143,6 @@
     <t>Pet Releaf</t>
   </si>
   <si>
-    <t>8100 Southpark Way</t>
-  </si>
-  <si>
-    <t>Unit A1</t>
-  </si>
-  <si>
     <t>Littleton</t>
   </si>
   <si>
@@ -189,12 +162,27 @@
   </si>
   <si>
     <t>UPS</t>
+  </si>
+  <si>
+    <t>Admin Contact</t>
+  </si>
+  <si>
+    <t>Admin Phone #</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>8100 Southpark way</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -217,7 +205,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,8 +242,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -273,54 +267,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -371,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -390,67 +336,50 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,9 +399,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -510,9 +439,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -545,26 +474,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -597,26 +509,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -789,11 +684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -813,12 +708,14 @@
   <sheetData>
     <row r="1" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="D1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="15"/>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
@@ -827,12 +724,14 @@
       <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="D2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -840,147 +739,141 @@
       <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
+        <v>5</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
+        <v>13</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
+        <v>6</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="19"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="19"/>
+        <v>8</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="12"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -989,16 +882,16 @@
       <c r="A11" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="22" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="20"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -1006,22 +899,20 @@
     </row>
     <row r="12" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="24"/>
+        <v>24</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -1029,20 +920,18 @@
     </row>
     <row r="13" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>48</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -1050,121 +939,115 @@
     </row>
     <row r="14" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>49</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="10"/>
       <c r="H14" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>6</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="20"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="29" t="s">
+      <c r="A17" s="19"/>
+      <c r="B17" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="29" t="s">
-        <v>27</v>
+      <c r="C17" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="21" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="33" t="s">
+      <c r="A18" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="K18" s="33" t="s">
-        <v>28</v>
+      <c r="B18" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1220,7 +1103,6 @@
       <c r="K22" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection password="CCF9" sheet="1"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1230,7 +1112,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1244,7 +1126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1258,12 +1140,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e752113-b2fb-4b78-ae69-b10b93a6ace4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1508,20 +1392,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4e752113-b2fb-4b78-ae69-b10b93a6ace4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF4FA091-CFE1-47AD-BE97-92BE82D1F85E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{568173AF-1203-46A5-BD75-373096ABAE85}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4e752113-b2fb-4b78-ae69-b10b93a6ace4"/>
+    <ds:schemaRef ds:uri="a2a82fc2-af7c-43c6-84e4-151c3b8f78f4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1546,10 +1431,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{568173AF-1203-46A5-BD75-373096ABAE85}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF4FA091-CFE1-47AD-BE97-92BE82D1F85E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>